<commit_message>
noted data I used in simulation for ease
</commit_message>
<xml_diff>
--- a/data/japan_costs/solar_japan.xlsx
+++ b/data/japan_costs/solar_japan.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="55">
   <si>
     <t>r12</t>
   </si>
@@ -286,6 +286,10 @@
   </si>
   <si>
     <t>Innvestment cost and O&amp;M cost are shown in the figure as annotation</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>*used in simulation</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -993,8 +997,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B6" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="B11" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14:F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
@@ -1003,7 +1007,7 @@
     <col min="5" max="5" width="9.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B2">
         <v>1</v>
       </c>
@@ -1014,32 +1018,32 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="D3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="D4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="D5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="D6" s="4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="D7" s="11" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -1047,7 +1051,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A12">
         <v>1</v>
       </c>
@@ -1058,12 +1062,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C13" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C14" s="7" t="s">
         <v>49</v>
       </c>
@@ -1072,8 +1076,11 @@
         <f>2.2*10^3</f>
         <v>2200</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F14" s="11" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C15" s="8" t="s">
         <v>51</v>
       </c>
@@ -1081,6 +1088,9 @@
       <c r="E15" s="8">
         <f>56*1000000/1000000</f>
         <v>56</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.55000000000000004">

</xml_diff>